<commit_message>
Added verification of operating systems.
</commit_message>
<xml_diff>
--- a/15C-Red-BOM-2015-10-21.xlsx
+++ b/15C-Red-BOM-2015-10-21.xlsx
@@ -74,15 +74,6 @@
     <t>Lancer FW</t>
   </si>
   <si>
-    <t>SLES11.3 32-bit</t>
-  </si>
-  <si>
-    <t>SLES11.3 64-bit</t>
-  </si>
-  <si>
-    <t>SLES11.3 Xen 64-bit</t>
-  </si>
-  <si>
     <t>OCe11102R-N2-X</t>
   </si>
   <si>
@@ -753,29 +744,8 @@
     <t>PkgSDK Name</t>
   </si>
   <si>
-    <t>RHEL6.6 KVM 64-bit</t>
-  </si>
-  <si>
-    <t>RHEL6.6 64-bit</t>
-  </si>
-  <si>
-    <t>RHEL7.1 64-bit</t>
-  </si>
-  <si>
-    <t>RHEL7.1 KVM 64-bit</t>
-  </si>
-  <si>
     <t>00D8549
 00JY809</t>
-  </si>
-  <si>
-    <t>SLES12.0 64-bit</t>
-  </si>
-  <si>
-    <t>SLES12.0 Xen 64-bit</t>
-  </si>
-  <si>
-    <t>RHEL6.6 32-bit</t>
   </si>
   <si>
     <t>Vmware ESXi 6.0</t>
@@ -983,24 +953,6 @@
   </si>
   <si>
     <t>Initial Red 15C BOM (review and implement each line item)</t>
-  </si>
-  <si>
-    <t>RHEL6.7 32-bit</t>
-  </si>
-  <si>
-    <t>RHEL6.7 64-bit</t>
-  </si>
-  <si>
-    <t>RHEL6.7 KVM 64-bit</t>
-  </si>
-  <si>
-    <t>SLES11.4 32-bit</t>
-  </si>
-  <si>
-    <t>SLES11.4 64-bit</t>
-  </si>
-  <si>
-    <t>SLES11.4 Xen 64-bit</t>
   </si>
   <si>
     <t>SkyBird (2x10)</t>
@@ -1407,18 +1359,6 @@
     <t>Added elx_Gold_P2_N, elx_Gold_P2_I, elx_Gold_P2_F, elx_Gold_Plus_P2_N,  elx_Gold_Plus_P2_I, and elx_Gold_Plus_P2_F to columns N-X</t>
   </si>
   <si>
-    <t>RHEL7.2 64-bit</t>
-  </si>
-  <si>
-    <t>RHEL7.2 KVM 64-bit</t>
-  </si>
-  <si>
-    <t>SLES12.1 64-bit</t>
-  </si>
-  <si>
-    <t>SLES12.1 Xen 64-bit</t>
-  </si>
-  <si>
     <t>VMware ESXi 5.1 U3
 (Lenovo Customized Image)</t>
   </si>
@@ -1492,6 +1432,66 @@
   </si>
   <si>
     <t>Temp</t>
+  </si>
+  <si>
+    <t>RHEL 6.6 32-bit</t>
+  </si>
+  <si>
+    <t>RHEL 6.7 32-bit</t>
+  </si>
+  <si>
+    <t>RHEL 6.6 64-bit</t>
+  </si>
+  <si>
+    <t>RHEL 6.7 64-bit</t>
+  </si>
+  <si>
+    <t>RHEL 6.6 KVM 64-bit</t>
+  </si>
+  <si>
+    <t>RHEL 6.7 KVM 64-bit</t>
+  </si>
+  <si>
+    <t>RHEL 7.1 64-bit</t>
+  </si>
+  <si>
+    <t>RHEL 7.2 64-bit</t>
+  </si>
+  <si>
+    <t>RHEL 7.1 KVM 64-bit</t>
+  </si>
+  <si>
+    <t>RHEL 7.2 KVM 64-bit</t>
+  </si>
+  <si>
+    <t>SLES 11.3 32-bit</t>
+  </si>
+  <si>
+    <t>SLES 11.4 32-bit</t>
+  </si>
+  <si>
+    <t>SLES 11.3 64-bit</t>
+  </si>
+  <si>
+    <t>SLES 11.4 64-bit</t>
+  </si>
+  <si>
+    <t>SLES 11.3 Xen 64-bit</t>
+  </si>
+  <si>
+    <t>SLES 11.4 Xen 64-bit</t>
+  </si>
+  <si>
+    <t>SLES 12.0 64-bit</t>
+  </si>
+  <si>
+    <t>SLES 12.0 Xen 64-bit</t>
+  </si>
+  <si>
+    <t>SLES 12.1 64-bit</t>
+  </si>
+  <si>
+    <t>SLES 12.1 Xen 64-bit</t>
   </si>
 </sst>
 </file>
@@ -2234,27 +2234,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2295,6 +2274,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2306,6 +2294,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="196">
@@ -2805,8 +2805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2839,55 +2839,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
-        <v>397</v>
-      </c>
-      <c r="B1" s="119"/>
+      <c r="A1" s="112" t="s">
+        <v>377</v>
+      </c>
+      <c r="B1" s="112"/>
       <c r="C1" s="110"/>
       <c r="D1" s="110"/>
     </row>
     <row r="2" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="119" t="s">
-        <v>398</v>
-      </c>
-      <c r="B2" s="119"/>
+      <c r="A2" s="112" t="s">
+        <v>378</v>
+      </c>
+      <c r="B2" s="112"/>
     </row>
     <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="118" t="s">
-        <v>401</v>
-      </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
+      <c r="D4" s="136" t="s">
+        <v>381</v>
+      </c>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="112" t="s">
+      <c r="H4" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="113"/>
-      <c r="J4" s="113"/>
-      <c r="K4" s="113"/>
-      <c r="L4" s="114"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="134"/>
+      <c r="L4" s="135"/>
       <c r="M4" s="14"/>
-      <c r="N4" s="112" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="113"/>
-      <c r="P4" s="113"/>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="113"/>
-      <c r="S4" s="113"/>
-      <c r="T4" s="113"/>
-      <c r="U4" s="113"/>
-      <c r="V4" s="113"/>
-      <c r="W4" s="113"/>
-      <c r="X4" s="114"/>
+      <c r="N4" s="133" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="134"/>
+      <c r="P4" s="134"/>
+      <c r="Q4" s="134"/>
+      <c r="R4" s="134"/>
+      <c r="S4" s="134"/>
+      <c r="T4" s="134"/>
+      <c r="U4" s="134"/>
+      <c r="V4" s="134"/>
+      <c r="W4" s="134"/>
+      <c r="X4" s="135"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B5" s="88" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
@@ -2904,38 +2904,38 @@
         <v>7</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>4</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M5" s="20"/>
       <c r="N5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="R5" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="P5" s="21" t="s">
+      <c r="S5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="T5" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="R5" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="S5" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="T5" s="21" t="s">
-        <v>49</v>
       </c>
       <c r="U5" s="21" t="s">
         <v>12</v>
@@ -2944,30 +2944,30 @@
         <v>13</v>
       </c>
       <c r="W5" s="22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="X5" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B6" s="89" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="115" t="s">
+      <c r="D6" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="116"/>
-      <c r="F6" s="117"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="128"/>
       <c r="G6" s="23"/>
-      <c r="H6" s="115" t="s">
-        <v>208</v>
-      </c>
-      <c r="I6" s="116"/>
-      <c r="J6" s="116"/>
-      <c r="K6" s="116"/>
-      <c r="L6" s="117"/>
+      <c r="H6" s="126" t="s">
+        <v>205</v>
+      </c>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="128"/>
       <c r="M6" s="24"/>
       <c r="N6" s="97" t="s">
         <v>9</v>
@@ -2976,7 +2976,7 @@
         <v>10</v>
       </c>
       <c r="P6" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Q6" s="84" t="s">
         <v>11</v>
@@ -2994,24 +2994,24 @@
         <v>8</v>
       </c>
       <c r="V6" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="W6" s="84" t="s">
         <v>9</v>
       </c>
       <c r="X6" s="97" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="Y6" s="76"/>
       <c r="Z6" s="25"/>
     </row>
     <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B7" s="90" t="s">
-        <v>238</v>
+        <v>394</v>
       </c>
       <c r="C7" s="26"/>
       <c r="D7" s="27" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E7" s="28">
         <v>5464</v>
@@ -3021,64 +3021,64 @@
       </c>
       <c r="G7" s="30"/>
       <c r="H7" s="98" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="I7" s="95" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J7" s="96" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K7" s="95" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L7" s="95" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M7" s="24"/>
       <c r="N7" s="97" t="s">
         <v>10</v>
       </c>
       <c r="O7" s="97" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="P7" s="83" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="Q7" s="97" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="R7" s="97" t="s">
         <v>10</v>
       </c>
       <c r="S7" s="97" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="T7" s="97" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="U7" s="97" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="V7" s="83" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="W7" s="97" t="s">
         <v>10</v>
       </c>
       <c r="X7" s="97" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Y7" s="76"/>
       <c r="Z7" s="32"/>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B8" s="90" t="s">
-        <v>302</v>
+        <v>395</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E8" s="33">
         <v>5463</v>
@@ -3088,61 +3088,61 @@
       </c>
       <c r="G8" s="35"/>
       <c r="H8" s="98" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="I8" s="41" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="J8" s="41" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="K8" s="40" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="L8" s="40" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="N8" s="97" t="s">
         <v>11</v>
       </c>
       <c r="O8" s="41" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="P8" s="83" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="Q8" s="41" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="R8" s="97" t="s">
         <v>11</v>
       </c>
       <c r="S8" s="41" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="T8" s="41" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="U8" s="86"/>
       <c r="V8" s="83" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="W8" s="97" t="s">
         <v>11</v>
       </c>
       <c r="X8" s="97" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Y8" s="76"/>
       <c r="Z8" s="32"/>
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B9" s="92" t="s">
-        <v>232</v>
+        <v>396</v>
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="27" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E9" s="37">
         <v>5462</v>
@@ -3152,256 +3152,256 @@
       </c>
       <c r="G9" s="35"/>
       <c r="H9" s="111" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="I9" s="41" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="K9" s="41" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="L9" s="40" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="N9" s="64" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="O9" s="85" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P9" s="83" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="Q9" s="97" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="R9" s="97" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="S9" s="85" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="T9" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="U9" s="86"/>
       <c r="V9" s="83" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="W9" s="97" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="X9" s="97" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="Y9" s="76"/>
       <c r="Z9" s="32"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B10" s="90" t="s">
-        <v>303</v>
+        <v>397</v>
       </c>
       <c r="C10" s="36"/>
       <c r="D10" s="15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="F10" s="38">
         <v>4</v>
       </c>
       <c r="G10" s="35"/>
       <c r="N10" s="64" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="O10" s="97" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="P10" s="84" t="s">
         <v>8</v>
       </c>
       <c r="Q10" s="97" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="R10" s="64" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="S10" s="97" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="T10" s="83" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="U10" s="86"/>
       <c r="V10" s="86"/>
       <c r="W10" s="97" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="X10" s="97" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="Y10" s="76"/>
       <c r="Z10" s="32"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B11" s="92" t="s">
-        <v>231</v>
+        <v>398</v>
       </c>
       <c r="C11" s="36"/>
       <c r="D11" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="F11" s="29">
         <v>5</v>
       </c>
       <c r="G11" s="39"/>
-      <c r="H11" s="115" t="s">
-        <v>209</v>
-      </c>
-      <c r="I11" s="116"/>
-      <c r="J11" s="116"/>
-      <c r="K11" s="116"/>
-      <c r="L11" s="117"/>
+      <c r="H11" s="126" t="s">
+        <v>206</v>
+      </c>
+      <c r="I11" s="127"/>
+      <c r="J11" s="127"/>
+      <c r="K11" s="127"/>
+      <c r="L11" s="128"/>
       <c r="N11" s="64" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="O11" s="85" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P11" s="64" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="Q11" s="97" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="R11" s="64" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="S11" s="85" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="T11" s="83" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="U11" s="86"/>
       <c r="V11" s="86"/>
       <c r="W11" s="97" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="X11" s="97" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="Y11" s="76"/>
       <c r="Z11" s="32"/>
     </row>
     <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B12" s="90" t="s">
-        <v>304</v>
+        <v>399</v>
       </c>
       <c r="C12" s="36"/>
       <c r="D12" s="27" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="F12" s="29">
         <v>6</v>
       </c>
       <c r="G12" s="30"/>
-      <c r="H12" s="124" t="s">
-        <v>333</v>
+      <c r="H12" s="117" t="s">
+        <v>317</v>
       </c>
       <c r="I12" s="95" t="s">
+        <v>178</v>
+      </c>
+      <c r="J12" s="96" t="s">
+        <v>179</v>
+      </c>
+      <c r="K12" s="95" t="s">
+        <v>180</v>
+      </c>
+      <c r="L12" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="J12" s="96" t="s">
-        <v>182</v>
-      </c>
-      <c r="K12" s="95" t="s">
-        <v>183</v>
-      </c>
-      <c r="L12" s="95" t="s">
-        <v>184</v>
-      </c>
       <c r="N12" s="41" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="O12" s="97" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="Q12" s="97" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="R12" s="41" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="S12" s="97" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="T12" s="83" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="U12" s="86"/>
       <c r="V12" s="86"/>
       <c r="W12" s="96" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="X12" s="97" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Y12" s="76"/>
       <c r="Z12" s="32"/>
     </row>
     <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B13" s="90" t="s">
-        <v>233</v>
+        <v>400</v>
       </c>
       <c r="C13" s="36"/>
       <c r="D13" s="41" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="F13" s="45">
         <v>7</v>
       </c>
       <c r="G13" s="30"/>
-      <c r="H13" s="136"/>
+      <c r="H13" s="132"/>
       <c r="I13" s="95" t="s">
+        <v>182</v>
+      </c>
+      <c r="J13" s="96" t="s">
+        <v>183</v>
+      </c>
+      <c r="K13" s="95" t="s">
+        <v>184</v>
+      </c>
+      <c r="L13" s="95" t="s">
         <v>185</v>
       </c>
-      <c r="J13" s="96" t="s">
-        <v>186</v>
-      </c>
-      <c r="K13" s="95" t="s">
-        <v>187</v>
-      </c>
-      <c r="L13" s="95" t="s">
-        <v>188</v>
-      </c>
       <c r="N13" s="41" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="O13" s="85" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="Q13" s="97" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="R13" s="41" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="S13" s="85" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="T13" s="97" t="s">
         <v>8</v>
@@ -3409,21 +3409,21 @@
       <c r="U13" s="86"/>
       <c r="V13" s="86"/>
       <c r="W13" s="96" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="X13" s="97" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Y13" s="76"/>
       <c r="Z13" s="32"/>
     </row>
     <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B14" s="90" t="s">
-        <v>386</v>
+        <v>401</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E14" s="33">
         <v>8869</v>
@@ -3431,56 +3431,56 @@
       <c r="F14" s="34">
         <v>8</v>
       </c>
-      <c r="H14" s="136"/>
+      <c r="H14" s="132"/>
       <c r="I14" s="105" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J14" s="106" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K14" s="105" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L14" s="105" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="N14" s="41" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="O14" s="85" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="P14" s="86"/>
       <c r="Q14" s="97" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="R14" s="41" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="S14" s="85" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="T14" s="64" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="U14" s="86"/>
       <c r="V14" s="86"/>
       <c r="W14" s="96" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="X14" s="97" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Y14" s="76"/>
       <c r="Z14" s="32"/>
     </row>
     <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B15" s="92" t="s">
-        <v>234</v>
+        <v>402</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="27" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E15" s="37">
         <v>8872</v>
@@ -3488,53 +3488,53 @@
       <c r="F15" s="29">
         <v>9</v>
       </c>
-      <c r="H15" s="125"/>
+      <c r="H15" s="118"/>
       <c r="I15" s="95" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="J15" s="96" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="K15" s="95" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="L15" s="95" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="N15" s="97" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="O15" s="97" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="P15" s="86"/>
       <c r="Q15" s="97" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="R15" s="97" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="S15" s="97" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="T15" s="97" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="U15" s="86"/>
       <c r="V15" s="86"/>
       <c r="X15" s="97" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="Y15" s="76"/>
       <c r="Z15" s="32"/>
     </row>
     <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B16" s="92" t="s">
-        <v>387</v>
+        <v>403</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="27" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="E16" s="37">
         <v>1234</v>
@@ -3542,54 +3542,54 @@
       <c r="F16" s="29">
         <v>10</v>
       </c>
-      <c r="H16" s="124" t="s">
-        <v>411</v>
+      <c r="H16" s="117" t="s">
+        <v>391</v>
       </c>
       <c r="I16" s="40" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="J16" s="96" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="K16" s="40" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="L16" s="40" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="N16" s="97" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="O16" s="97" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="P16" s="86"/>
       <c r="Q16" s="97" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="R16" s="97" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S16" s="97" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="T16" s="97" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="V16" s="86"/>
       <c r="X16" s="97" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="Y16" s="76"/>
       <c r="Z16" s="32"/>
     </row>
     <row r="17" spans="2:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B17" s="91" t="s">
-        <v>14</v>
+        <v>404</v>
       </c>
       <c r="C17" s="47"/>
       <c r="D17" s="27" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="E17" s="37">
         <v>4321</v>
@@ -3598,534 +3598,534 @@
         <v>11</v>
       </c>
       <c r="G17" s="76"/>
-      <c r="H17" s="125"/>
+      <c r="H17" s="118"/>
       <c r="I17" s="40" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="J17" s="96" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="K17" s="40" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="L17" s="40" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="N17" s="97" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O17" s="97" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="P17" s="86"/>
       <c r="Q17" s="97" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="R17" s="97" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S17" s="97" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="T17" s="97" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="V17" s="86"/>
       <c r="X17" s="97" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="Y17" s="76"/>
       <c r="Z17" s="32"/>
     </row>
     <row r="18" spans="2:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B18" s="90" t="s">
-        <v>305</v>
+        <v>405</v>
       </c>
       <c r="C18" s="8"/>
       <c r="G18" s="76"/>
-      <c r="H18" s="126" t="s">
-        <v>409</v>
+      <c r="H18" s="119" t="s">
+        <v>389</v>
       </c>
       <c r="I18" s="40" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="J18" s="41" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="K18" s="40" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="L18" s="40" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="N18" s="97" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="O18" s="97" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="P18" s="86"/>
       <c r="Q18" s="97" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="R18" s="97" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="S18" s="97" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="T18" s="97" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="V18" s="86"/>
       <c r="W18" s="87"/>
       <c r="X18" s="97" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Y18" s="76"/>
       <c r="Z18" s="32"/>
     </row>
     <row r="19" spans="2:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B19" s="91" t="s">
-        <v>15</v>
+        <v>406</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="133" t="s">
-        <v>252</v>
-      </c>
-      <c r="E19" s="134"/>
-      <c r="F19" s="135"/>
+      <c r="D19" s="129" t="s">
+        <v>242</v>
+      </c>
+      <c r="E19" s="130"/>
+      <c r="F19" s="131"/>
       <c r="G19" s="76"/>
-      <c r="H19" s="127"/>
+      <c r="H19" s="120"/>
       <c r="I19" s="40" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="J19" s="41" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="K19" s="40" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="L19" s="40" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="N19" s="97" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="O19" s="64" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="P19" s="86"/>
       <c r="Q19" s="64" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="R19" s="97" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="S19" s="64" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="T19" s="97" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="V19" s="86"/>
       <c r="W19" s="87"/>
       <c r="X19" s="97" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="Y19" s="76"/>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B20" s="90" t="s">
-        <v>306</v>
+        <v>407</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="41" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="E20" s="79" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="F20" s="45">
         <v>50</v>
       </c>
       <c r="G20" s="76"/>
       <c r="N20" s="97" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="O20" s="41" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="P20" s="86"/>
       <c r="Q20" s="41" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="R20" s="97" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="S20" s="41" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="T20" s="97" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="V20" s="86"/>
       <c r="W20" s="87"/>
       <c r="X20" s="97" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Y20" s="76"/>
     </row>
     <row r="21" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B21" s="92" t="s">
-        <v>16</v>
+        <v>408</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="41" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="F21" s="45">
         <v>51</v>
       </c>
-      <c r="H21" s="115" t="s">
-        <v>210</v>
-      </c>
-      <c r="I21" s="116"/>
-      <c r="J21" s="116"/>
-      <c r="K21" s="116"/>
-      <c r="L21" s="117"/>
+      <c r="H21" s="126" t="s">
+        <v>207</v>
+      </c>
+      <c r="I21" s="127"/>
+      <c r="J21" s="127"/>
+      <c r="K21" s="127"/>
+      <c r="L21" s="128"/>
       <c r="N21" s="97" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P21" s="86"/>
       <c r="Q21" s="76"/>
       <c r="R21" s="97" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="T21" s="97" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="U21" s="86"/>
       <c r="V21" s="86"/>
       <c r="W21" s="87"/>
       <c r="X21" s="97" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="Y21" s="76"/>
     </row>
     <row r="22" spans="2:26" ht="45" x14ac:dyDescent="0.2">
       <c r="B22" s="90" t="s">
-        <v>307</v>
+        <v>409</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="41" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="F22" s="80">
         <v>52</v>
       </c>
-      <c r="H22" s="128" t="s">
-        <v>333</v>
+      <c r="H22" s="121" t="s">
+        <v>317</v>
       </c>
       <c r="I22" s="95" t="s">
+        <v>189</v>
+      </c>
+      <c r="J22" s="96" t="s">
+        <v>190</v>
+      </c>
+      <c r="K22" s="95" t="s">
+        <v>191</v>
+      </c>
+      <c r="L22" s="95" t="s">
         <v>192</v>
       </c>
-      <c r="J22" s="96" t="s">
-        <v>193</v>
-      </c>
-      <c r="K22" s="95" t="s">
-        <v>194</v>
-      </c>
-      <c r="L22" s="95" t="s">
-        <v>195</v>
-      </c>
       <c r="N22" s="97" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P22" s="86"/>
       <c r="Q22" s="76"/>
       <c r="R22" s="97" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="S22" s="87"/>
       <c r="T22" s="97" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="U22" s="86"/>
       <c r="V22" s="86"/>
       <c r="W22" s="87"/>
       <c r="X22" s="97" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Y22" s="76"/>
     </row>
     <row r="23" spans="2:26" ht="45" x14ac:dyDescent="0.2">
       <c r="B23" s="92" t="s">
-        <v>236</v>
+        <v>410</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="64" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="E23" s="44" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="F23" s="81">
         <v>53</v>
       </c>
-      <c r="H23" s="129"/>
+      <c r="H23" s="122"/>
       <c r="I23" s="95" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J23" s="96" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K23" s="95" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L23" s="95" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N23" s="97" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="P23" s="86"/>
       <c r="Q23" s="76"/>
       <c r="R23" s="97" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="S23" s="87"/>
       <c r="T23" s="97" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="U23" s="86"/>
       <c r="V23" s="86"/>
       <c r="W23" s="87"/>
       <c r="X23" s="97" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="Y23" s="76"/>
     </row>
     <row r="24" spans="2:26" ht="45" x14ac:dyDescent="0.2">
       <c r="B24" s="92" t="s">
-        <v>237</v>
+        <v>411</v>
       </c>
       <c r="C24" s="8"/>
       <c r="H24" s="104" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="I24" s="41" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="J24" s="41" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="K24" s="40" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="L24" s="40" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="N24" s="97" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="P24" s="86"/>
       <c r="Q24" s="86"/>
       <c r="R24" s="97" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="S24" s="86"/>
       <c r="T24" s="97" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="U24" s="86"/>
       <c r="V24" s="86"/>
       <c r="W24" s="87"/>
       <c r="X24" s="97" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="Y24" s="76"/>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B25" s="92" t="s">
-        <v>388</v>
+        <v>412</v>
       </c>
       <c r="D25" s="46"/>
       <c r="E25" s="7"/>
       <c r="F25" s="48"/>
       <c r="N25" s="97" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="P25" s="86"/>
       <c r="Q25" s="86"/>
       <c r="R25" s="97" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="S25" s="86"/>
       <c r="T25" s="64" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="U25" s="86"/>
       <c r="V25" s="86"/>
       <c r="W25" s="87"/>
       <c r="X25" s="97" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="Y25" s="76"/>
     </row>
     <row r="26" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B26" s="92" t="s">
-        <v>389</v>
+        <v>413</v>
       </c>
       <c r="D26" s="46"/>
       <c r="E26" s="7"/>
       <c r="F26" s="48"/>
-      <c r="H26" s="115" t="s">
-        <v>211</v>
-      </c>
-      <c r="I26" s="116"/>
-      <c r="J26" s="116"/>
-      <c r="K26" s="116"/>
-      <c r="L26" s="117"/>
+      <c r="H26" s="126" t="s">
+        <v>208</v>
+      </c>
+      <c r="I26" s="127"/>
+      <c r="J26" s="127"/>
+      <c r="K26" s="127"/>
+      <c r="L26" s="128"/>
       <c r="N26" s="97" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="O26" s="49"/>
       <c r="P26" s="86"/>
       <c r="Q26" s="86"/>
       <c r="R26" s="97" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="S26" s="86"/>
       <c r="T26" s="41" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="U26" s="86"/>
       <c r="V26" s="86"/>
       <c r="W26" s="87"/>
       <c r="X26" s="97" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="Y26" s="76"/>
     </row>
     <row r="27" spans="2:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B27" s="90" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="48"/>
-      <c r="H27" s="130" t="s">
-        <v>333</v>
+      <c r="H27" s="123" t="s">
+        <v>317</v>
       </c>
       <c r="I27" s="95" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J27" s="96" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K27" s="95" t="s">
+        <v>56</v>
+      </c>
+      <c r="L27" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="L27" s="95" t="s">
-        <v>62</v>
-      </c>
       <c r="N27" s="97" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O27" s="49"/>
       <c r="P27" s="86"/>
       <c r="Q27" s="86"/>
       <c r="R27" s="97" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="S27" s="86"/>
       <c r="U27" s="86"/>
       <c r="V27" s="86"/>
       <c r="W27" s="76"/>
       <c r="X27" s="97" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="Y27" s="76"/>
     </row>
     <row r="28" spans="2:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B28" s="50" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="D28" s="71"/>
       <c r="E28" s="67"/>
       <c r="F28" s="72"/>
-      <c r="H28" s="131"/>
+      <c r="H28" s="124"/>
       <c r="I28" s="96" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="J28" s="96" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K28" s="95" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="L28" s="95" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="N28" s="97" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O28" s="42"/>
       <c r="P28" s="86"/>
       <c r="Q28" s="25"/>
       <c r="R28" s="97" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="S28" s="25"/>
       <c r="U28" s="86"/>
       <c r="V28" s="86"/>
       <c r="W28" s="76"/>
       <c r="X28" s="97" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="Y28" s="76"/>
     </row>
     <row r="29" spans="2:26" ht="30" x14ac:dyDescent="0.2">
       <c r="B29" s="92" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="D29" s="71"/>
       <c r="E29" s="67"/>
       <c r="F29" s="72"/>
-      <c r="H29" s="131"/>
+      <c r="H29" s="124"/>
       <c r="I29" s="95" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J29" s="96" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K29" s="95" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L29" s="95" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N29" s="97" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O29" s="69"/>
       <c r="P29" s="25"/>
       <c r="Q29" s="68"/>
       <c r="R29" s="97" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="S29" s="68"/>
       <c r="T29" s="68"/>
       <c r="U29" s="25"/>
       <c r="V29" s="25"/>
       <c r="X29" s="97" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="2:26" s="66" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -4133,135 +4133,135 @@
       <c r="D30" s="46"/>
       <c r="E30" s="7"/>
       <c r="F30" s="48"/>
-      <c r="H30" s="131"/>
+      <c r="H30" s="124"/>
       <c r="I30" s="96" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="J30" s="96" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K30" s="95" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="L30" s="95" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="N30" s="97" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="O30" s="69"/>
       <c r="P30" s="68"/>
       <c r="Q30" s="68"/>
       <c r="R30" s="97" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="S30" s="68"/>
       <c r="T30" s="68"/>
       <c r="U30" s="68"/>
       <c r="V30" s="68"/>
       <c r="X30" s="97" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" spans="2:26" s="66" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="D31" s="46"/>
       <c r="E31" s="7"/>
       <c r="F31" s="48"/>
-      <c r="H31" s="132"/>
+      <c r="H31" s="125"/>
       <c r="I31" s="96" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J31" s="96" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K31" s="95" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="L31" s="95" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="N31" s="97" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O31" s="42"/>
       <c r="P31" s="68"/>
       <c r="Q31" s="25"/>
       <c r="R31" s="97" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="68"/>
       <c r="V31" s="68"/>
       <c r="X31" s="97" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" spans="2:26" ht="60" x14ac:dyDescent="0.2">
       <c r="D32" s="46"/>
       <c r="E32" s="7"/>
       <c r="F32" s="48"/>
-      <c r="H32" s="120" t="s">
-        <v>365</v>
+      <c r="H32" s="113" t="s">
+        <v>349</v>
       </c>
       <c r="I32" s="96" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J32" s="96" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K32" s="95" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="L32" s="95" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="N32" s="97" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
       <c r="Q32" s="25"/>
       <c r="R32" s="97" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="T32" s="25"/>
       <c r="U32" s="25"/>
       <c r="V32" s="25"/>
       <c r="X32" s="97" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" spans="4:24" ht="30" x14ac:dyDescent="0.2">
       <c r="D33" s="46"/>
       <c r="E33" s="7"/>
       <c r="F33" s="48"/>
-      <c r="H33" s="121"/>
+      <c r="H33" s="114"/>
       <c r="I33" s="96" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="J33" s="96" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K33" s="95" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="L33" s="95" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="M33" s="25"/>
       <c r="N33" s="97" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="P33" s="25"/>
       <c r="Q33" s="25"/>
       <c r="R33" s="97" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="S33" s="25"/>
       <c r="T33" s="25"/>
       <c r="X33" s="97" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="4:24" ht="30" x14ac:dyDescent="0.2">
@@ -4269,102 +4269,102 @@
       <c r="E34" s="7"/>
       <c r="F34" s="48"/>
       <c r="H34" s="82" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="I34" s="41" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="J34" s="41" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="K34" s="40" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="L34" s="40" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="N34" s="97" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="P34" s="25"/>
       <c r="Q34" s="25"/>
       <c r="R34" s="97" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="S34" s="25"/>
       <c r="T34" s="25"/>
       <c r="U34" s="25"/>
       <c r="V34" s="25"/>
       <c r="X34" s="97" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="4:24" ht="30" x14ac:dyDescent="0.2">
       <c r="D35" s="46"/>
       <c r="E35" s="7"/>
       <c r="F35" s="48"/>
-      <c r="H35" s="122" t="s">
-        <v>412</v>
+      <c r="H35" s="115" t="s">
+        <v>392</v>
       </c>
       <c r="I35" s="96" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="J35" s="94" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="K35" s="94" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="L35" s="99" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="N35" s="97" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="P35" s="25"/>
       <c r="Q35" s="25"/>
       <c r="R35" s="97" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="S35" s="25"/>
       <c r="T35" s="25"/>
       <c r="U35" s="25"/>
       <c r="V35" s="25"/>
       <c r="X35" s="97" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" spans="4:24" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D36" s="51"/>
       <c r="E36" s="6"/>
       <c r="F36" s="52"/>
-      <c r="H36" s="123"/>
+      <c r="H36" s="116"/>
       <c r="I36" s="96" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="J36" s="94" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="K36" s="94" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="L36" s="99" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="N36" s="64" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="P36" s="25"/>
       <c r="Q36" s="25"/>
       <c r="R36" s="64" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="S36" s="25"/>
       <c r="T36" s="25"/>
       <c r="U36" s="25"/>
       <c r="V36" s="25"/>
       <c r="X36" s="64" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="4:24" ht="30" x14ac:dyDescent="0.2">
@@ -4372,33 +4372,33 @@
       <c r="E37" s="7"/>
       <c r="F37" s="52"/>
       <c r="H37" s="82" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="I37" s="41" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="J37" s="41" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="K37" s="40" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="L37" s="40" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="N37" s="64" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="64" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="S37" s="25"/>
       <c r="T37" s="25"/>
       <c r="U37" s="25"/>
       <c r="V37" s="25"/>
       <c r="X37" s="64" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="38" spans="4:24" ht="30" x14ac:dyDescent="0.2">
@@ -4406,23 +4406,23 @@
         <v>53</v>
       </c>
       <c r="I38" s="41" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="J38" s="41" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="K38" s="95" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="L38" s="100" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="N38" s="64" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="Q38" s="25"/>
       <c r="R38" s="64" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="S38" s="25"/>
       <c r="T38" s="25"/>
@@ -4430,16 +4430,16 @@
       <c r="V38" s="25"/>
       <c r="W38" s="42"/>
       <c r="X38" s="64" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="39" spans="4:24" x14ac:dyDescent="0.2">
       <c r="N39" s="97" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="97" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="S39" s="25"/>
       <c r="T39" s="25"/>
@@ -4447,16 +4447,16 @@
       <c r="V39" s="25"/>
       <c r="W39" s="42"/>
       <c r="X39" s="41" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="4:24" x14ac:dyDescent="0.2">
       <c r="N40" s="97" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="Q40" s="25"/>
       <c r="R40" s="97" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="S40" s="25"/>
       <c r="T40" s="25"/>
@@ -4464,16 +4464,16 @@
       <c r="V40" s="25"/>
       <c r="W40" s="42"/>
       <c r="X40" s="41" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41" spans="4:24" x14ac:dyDescent="0.2">
       <c r="N41" s="97" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="Q41" s="25"/>
       <c r="R41" s="97" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="S41" s="25"/>
       <c r="T41" s="25"/>
@@ -4481,7 +4481,7 @@
       <c r="V41" s="25"/>
       <c r="W41" s="42"/>
       <c r="X41" s="41" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="42" spans="4:24" x14ac:dyDescent="0.2">
@@ -4491,12 +4491,12 @@
       <c r="K42" s="66"/>
       <c r="L42" s="66"/>
       <c r="N42" s="97" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="O42" s="25"/>
       <c r="Q42" s="25"/>
       <c r="R42" s="97" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="S42" s="25"/>
       <c r="T42" s="25"/>
@@ -4507,13 +4507,13 @@
     </row>
     <row r="43" spans="4:24" x14ac:dyDescent="0.2">
       <c r="N43" s="97" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="O43" s="25"/>
       <c r="P43" s="25"/>
       <c r="Q43" s="25"/>
       <c r="R43" s="97" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="S43" s="25"/>
       <c r="T43" s="25"/>
@@ -4530,13 +4530,13 @@
       <c r="K44" s="42"/>
       <c r="L44" s="25"/>
       <c r="N44" s="97" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="O44" s="25"/>
       <c r="P44" s="25"/>
       <c r="Q44" s="25"/>
       <c r="R44" s="97" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="S44" s="25"/>
       <c r="T44" s="25"/>
@@ -4550,13 +4550,13 @@
       <c r="E45" s="56"/>
       <c r="F45" s="57"/>
       <c r="N45" s="64" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="O45" s="25"/>
       <c r="P45" s="25"/>
       <c r="Q45" s="25"/>
       <c r="R45" s="64" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="S45" s="25"/>
       <c r="T45" s="25"/>
@@ -4570,13 +4570,13 @@
       <c r="E46" s="56"/>
       <c r="F46" s="57"/>
       <c r="N46" s="64" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="O46" s="25"/>
       <c r="P46" s="25"/>
       <c r="Q46" s="25"/>
       <c r="R46" s="64" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="S46" s="25"/>
       <c r="T46" s="25"/>
@@ -4590,13 +4590,13 @@
       <c r="E47" s="56"/>
       <c r="F47" s="57"/>
       <c r="N47" s="64" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="O47" s="25"/>
       <c r="P47" s="25"/>
       <c r="Q47" s="25"/>
       <c r="R47" s="64" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="S47" s="25"/>
       <c r="T47" s="25"/>
@@ -4610,13 +4610,13 @@
       <c r="E48" s="58"/>
       <c r="F48" s="57"/>
       <c r="N48" s="41" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="O48" s="25"/>
       <c r="P48" s="25"/>
       <c r="Q48" s="25"/>
       <c r="R48" s="41" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="S48" s="25"/>
       <c r="T48" s="25"/>
@@ -4630,13 +4630,13 @@
       <c r="E49" s="56"/>
       <c r="F49" s="57"/>
       <c r="N49" s="41" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="O49" s="25"/>
       <c r="P49" s="25"/>
       <c r="Q49" s="25"/>
       <c r="R49" s="41" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="S49" s="25"/>
       <c r="T49" s="25"/>
@@ -4647,13 +4647,13 @@
     </row>
     <row r="50" spans="4:24" x14ac:dyDescent="0.2">
       <c r="N50" s="41" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="O50" s="25"/>
       <c r="P50" s="25"/>
       <c r="Q50" s="25"/>
       <c r="R50" s="41" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="S50" s="25"/>
       <c r="T50" s="25"/>
@@ -4866,6 +4866,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="H32:H33"/>
@@ -4879,11 +4884,6 @@
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="H12:H15"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4907,16 +4907,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -4926,7 +4926,7 @@
       <c r="B2" s="107"/>
       <c r="C2" s="107"/>
       <c r="D2" s="73" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -4934,7 +4934,7 @@
       <c r="B3" s="107"/>
       <c r="C3" s="107"/>
       <c r="D3" s="73" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -4942,7 +4942,7 @@
       <c r="B4" s="107"/>
       <c r="C4" s="107"/>
       <c r="D4" s="73" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -4958,7 +4958,7 @@
       <c r="B6" s="107"/>
       <c r="C6" s="107"/>
       <c r="D6" s="73" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -4974,7 +4974,7 @@
       <c r="B8" s="107"/>
       <c r="C8" s="107"/>
       <c r="D8" s="73" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -4982,7 +4982,7 @@
       <c r="B9" s="107"/>
       <c r="C9" s="107"/>
       <c r="D9" s="73" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -4990,7 +4990,7 @@
       <c r="B10" s="107"/>
       <c r="C10" s="107"/>
       <c r="D10" s="73" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -4998,7 +4998,7 @@
       <c r="B11" s="107"/>
       <c r="C11" s="107"/>
       <c r="D11" s="73" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5016,7 +5016,7 @@
       </c>
       <c r="C13" s="107"/>
       <c r="D13" s="73" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5024,7 +5024,7 @@
       <c r="B14" s="107"/>
       <c r="C14" s="107"/>
       <c r="D14" s="73" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5042,7 +5042,7 @@
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="73" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5050,7 +5050,7 @@
       <c r="B17" s="107"/>
       <c r="C17" s="107"/>
       <c r="D17" s="73" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5058,7 +5058,7 @@
       <c r="B18" s="107"/>
       <c r="C18" s="107"/>
       <c r="D18" s="73" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5066,7 +5066,7 @@
       <c r="B19" s="107"/>
       <c r="C19" s="107"/>
       <c r="D19" s="73" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5074,7 +5074,7 @@
       <c r="B20" s="107"/>
       <c r="C20" s="107"/>
       <c r="D20" s="73" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5082,7 +5082,7 @@
       <c r="B21" s="107"/>
       <c r="C21" s="107"/>
       <c r="D21" s="73" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5090,7 +5090,7 @@
       <c r="B22" s="107"/>
       <c r="C22" s="107"/>
       <c r="D22" s="73" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5098,7 +5098,7 @@
       <c r="B23" s="107"/>
       <c r="C23" s="107"/>
       <c r="D23" s="73" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5106,7 +5106,7 @@
       <c r="B24" s="107"/>
       <c r="C24" s="107"/>
       <c r="D24" s="73" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5114,7 +5114,7 @@
       <c r="B25" s="107"/>
       <c r="C25" s="107"/>
       <c r="D25" s="73" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5122,7 +5122,7 @@
       <c r="B26" s="107"/>
       <c r="C26" s="107"/>
       <c r="D26" s="73" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
@@ -5139,10 +5139,10 @@
         <v>180639</v>
       </c>
       <c r="C28" s="77" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="D28" s="73" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
@@ -5255,702 +5255,702 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="101" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="102" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="103" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="103" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="93" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="93" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="93" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="103" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="103" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="103" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="93" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="93" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="93" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="103" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="103" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="103" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="93" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="93" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="93" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="103" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="103" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -5975,134 +5975,134 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B2" s="1">
         <v>203</v>
       </c>
       <c r="C2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B3" s="1">
         <v>208</v>
       </c>
       <c r="C3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B4" s="1">
         <v>209</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B5" s="1">
         <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="65" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B6" s="1">
         <v>210</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B7" s="1">
         <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1">
         <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1">
         <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B10" s="1">
         <v>311</v>
       </c>
       <c r="C10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B11" s="1">
         <v>312</v>
       </c>
       <c r="C11" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="65" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B12" s="1">
         <v>313</v>
       </c>
       <c r="C12" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More detailed parsing of OS list.
</commit_message>
<xml_diff>
--- a/15C-Red-BOM-2015-10-21.xlsx
+++ b/15C-Red-BOM-2015-10-21.xlsx
@@ -2234,6 +2234,27 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2274,15 +2295,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2294,18 +2306,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="196">
@@ -2806,7 +2806,7 @@
   <dimension ref="A1:Z76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2839,51 +2839,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="119" t="s">
         <v>377</v>
       </c>
-      <c r="B1" s="112"/>
+      <c r="B1" s="119"/>
       <c r="C1" s="110"/>
       <c r="D1" s="110"/>
     </row>
     <row r="2" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="119" t="s">
         <v>378</v>
       </c>
-      <c r="B2" s="112"/>
+      <c r="B2" s="119"/>
     </row>
     <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="136" t="s">
+      <c r="D4" s="118" t="s">
         <v>381</v>
       </c>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="133" t="s">
+      <c r="H4" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="134"/>
-      <c r="J4" s="134"/>
-      <c r="K4" s="134"/>
-      <c r="L4" s="135"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="114"/>
       <c r="M4" s="14"/>
-      <c r="N4" s="133" t="s">
+      <c r="N4" s="112" t="s">
         <v>53</v>
       </c>
-      <c r="O4" s="134"/>
-      <c r="P4" s="134"/>
-      <c r="Q4" s="134"/>
-      <c r="R4" s="134"/>
-      <c r="S4" s="134"/>
-      <c r="T4" s="134"/>
-      <c r="U4" s="134"/>
-      <c r="V4" s="134"/>
-      <c r="W4" s="134"/>
-      <c r="X4" s="135"/>
+      <c r="O4" s="113"/>
+      <c r="P4" s="113"/>
+      <c r="Q4" s="113"/>
+      <c r="R4" s="113"/>
+      <c r="S4" s="113"/>
+      <c r="T4" s="113"/>
+      <c r="U4" s="113"/>
+      <c r="V4" s="113"/>
+      <c r="W4" s="113"/>
+      <c r="X4" s="114"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B5" s="88" t="s">
@@ -2955,19 +2955,19 @@
         <v>47</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="126" t="s">
+      <c r="D6" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="127"/>
-      <c r="F6" s="128"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="117"/>
       <c r="G6" s="23"/>
-      <c r="H6" s="126" t="s">
+      <c r="H6" s="115" t="s">
         <v>205</v>
       </c>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="128"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="116"/>
+      <c r="K6" s="116"/>
+      <c r="L6" s="117"/>
       <c r="M6" s="24"/>
       <c r="N6" s="97" t="s">
         <v>9</v>
@@ -3262,13 +3262,13 @@
         <v>5</v>
       </c>
       <c r="G11" s="39"/>
-      <c r="H11" s="126" t="s">
+      <c r="H11" s="115" t="s">
         <v>206</v>
       </c>
-      <c r="I11" s="127"/>
-      <c r="J11" s="127"/>
-      <c r="K11" s="127"/>
-      <c r="L11" s="128"/>
+      <c r="I11" s="116"/>
+      <c r="J11" s="116"/>
+      <c r="K11" s="116"/>
+      <c r="L11" s="117"/>
       <c r="N11" s="64" t="s">
         <v>275</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="30"/>
-      <c r="H12" s="117" t="s">
+      <c r="H12" s="124" t="s">
         <v>317</v>
       </c>
       <c r="I12" s="95" t="s">
@@ -3375,7 +3375,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="30"/>
-      <c r="H13" s="132"/>
+      <c r="H13" s="136"/>
       <c r="I13" s="95" t="s">
         <v>182</v>
       </c>
@@ -3431,7 +3431,7 @@
       <c r="F14" s="34">
         <v>8</v>
       </c>
-      <c r="H14" s="132"/>
+      <c r="H14" s="136"/>
       <c r="I14" s="105" t="s">
         <v>186</v>
       </c>
@@ -3488,7 +3488,7 @@
       <c r="F15" s="29">
         <v>9</v>
       </c>
-      <c r="H15" s="118"/>
+      <c r="H15" s="125"/>
       <c r="I15" s="95" t="s">
         <v>188</v>
       </c>
@@ -3542,7 +3542,7 @@
       <c r="F16" s="29">
         <v>10</v>
       </c>
-      <c r="H16" s="117" t="s">
+      <c r="H16" s="124" t="s">
         <v>391</v>
       </c>
       <c r="I16" s="40" t="s">
@@ -3598,7 +3598,7 @@
         <v>11</v>
       </c>
       <c r="G17" s="76"/>
-      <c r="H17" s="118"/>
+      <c r="H17" s="125"/>
       <c r="I17" s="40" t="s">
         <v>258</v>
       </c>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="C18" s="8"/>
       <c r="G18" s="76"/>
-      <c r="H18" s="119" t="s">
+      <c r="H18" s="126" t="s">
         <v>389</v>
       </c>
       <c r="I18" s="40" t="s">
@@ -3690,13 +3690,13 @@
         <v>406</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="129" t="s">
+      <c r="D19" s="133" t="s">
         <v>242</v>
       </c>
-      <c r="E19" s="130"/>
-      <c r="F19" s="131"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="135"/>
       <c r="G19" s="76"/>
-      <c r="H19" s="120"/>
+      <c r="H19" s="127"/>
       <c r="I19" s="40" t="s">
         <v>260</v>
       </c>
@@ -3790,13 +3790,13 @@
       <c r="F21" s="45">
         <v>51</v>
       </c>
-      <c r="H21" s="126" t="s">
+      <c r="H21" s="115" t="s">
         <v>207</v>
       </c>
-      <c r="I21" s="127"/>
-      <c r="J21" s="127"/>
-      <c r="K21" s="127"/>
-      <c r="L21" s="128"/>
+      <c r="I21" s="116"/>
+      <c r="J21" s="116"/>
+      <c r="K21" s="116"/>
+      <c r="L21" s="117"/>
       <c r="N21" s="97" t="s">
         <v>74</v>
       </c>
@@ -3830,7 +3830,7 @@
       <c r="F22" s="80">
         <v>52</v>
       </c>
-      <c r="H22" s="121" t="s">
+      <c r="H22" s="128" t="s">
         <v>317</v>
       </c>
       <c r="I22" s="95" t="s">
@@ -3879,7 +3879,7 @@
       <c r="F23" s="81">
         <v>53</v>
       </c>
-      <c r="H23" s="122"/>
+      <c r="H23" s="129"/>
       <c r="I23" s="95" t="s">
         <v>193</v>
       </c>
@@ -3986,13 +3986,13 @@
       <c r="D26" s="46"/>
       <c r="E26" s="7"/>
       <c r="F26" s="48"/>
-      <c r="H26" s="126" t="s">
+      <c r="H26" s="115" t="s">
         <v>208</v>
       </c>
-      <c r="I26" s="127"/>
-      <c r="J26" s="127"/>
-      <c r="K26" s="127"/>
-      <c r="L26" s="128"/>
+      <c r="I26" s="116"/>
+      <c r="J26" s="116"/>
+      <c r="K26" s="116"/>
+      <c r="L26" s="117"/>
       <c r="N26" s="97" t="s">
         <v>367</v>
       </c>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="48"/>
-      <c r="H27" s="123" t="s">
+      <c r="H27" s="130" t="s">
         <v>317</v>
       </c>
       <c r="I27" s="95" t="s">
@@ -4060,7 +4060,7 @@
       <c r="D28" s="71"/>
       <c r="E28" s="67"/>
       <c r="F28" s="72"/>
-      <c r="H28" s="124"/>
+      <c r="H28" s="131"/>
       <c r="I28" s="96" t="s">
         <v>329</v>
       </c>
@@ -4098,7 +4098,7 @@
       <c r="D29" s="71"/>
       <c r="E29" s="67"/>
       <c r="F29" s="72"/>
-      <c r="H29" s="124"/>
+      <c r="H29" s="131"/>
       <c r="I29" s="95" t="s">
         <v>204</v>
       </c>
@@ -4133,7 +4133,7 @@
       <c r="D30" s="46"/>
       <c r="E30" s="7"/>
       <c r="F30" s="48"/>
-      <c r="H30" s="124"/>
+      <c r="H30" s="131"/>
       <c r="I30" s="96" t="s">
         <v>338</v>
       </c>
@@ -4167,7 +4167,7 @@
       <c r="D31" s="46"/>
       <c r="E31" s="7"/>
       <c r="F31" s="48"/>
-      <c r="H31" s="125"/>
+      <c r="H31" s="132"/>
       <c r="I31" s="96" t="s">
         <v>61</v>
       </c>
@@ -4201,7 +4201,7 @@
       <c r="D32" s="46"/>
       <c r="E32" s="7"/>
       <c r="F32" s="48"/>
-      <c r="H32" s="113" t="s">
+      <c r="H32" s="120" t="s">
         <v>349</v>
       </c>
       <c r="I32" s="96" t="s">
@@ -4236,7 +4236,7 @@
       <c r="D33" s="46"/>
       <c r="E33" s="7"/>
       <c r="F33" s="48"/>
-      <c r="H33" s="114"/>
+      <c r="H33" s="121"/>
       <c r="I33" s="96" t="s">
         <v>324</v>
       </c>
@@ -4303,7 +4303,7 @@
       <c r="D35" s="46"/>
       <c r="E35" s="7"/>
       <c r="F35" s="48"/>
-      <c r="H35" s="115" t="s">
+      <c r="H35" s="122" t="s">
         <v>392</v>
       </c>
       <c r="I35" s="96" t="s">
@@ -4338,7 +4338,7 @@
       <c r="D36" s="51"/>
       <c r="E36" s="6"/>
       <c r="F36" s="52"/>
-      <c r="H36" s="116"/>
+      <c r="H36" s="123"/>
       <c r="I36" s="96" t="s">
         <v>295</v>
       </c>
@@ -4866,11 +4866,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="H32:H33"/>
@@ -4884,6 +4879,11 @@
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="H12:H15"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>